<commit_message>
Fix rates in 1 and 5 [ref #4]
</commit_message>
<xml_diff>
--- a/doc/InOutEngine/1_with_out_exceptions.xlsx
+++ b/doc/InOutEngine/1_with_out_exceptions.xlsx
@@ -29,6 +29,7 @@
     <definedName function="false" hidden="false" name="_xlnm._FilterDatabase_1_1" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
     <definedName function="false" hidden="false" name="_xlnm._FilterDatabase_1_1_1" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
     <definedName function="false" hidden="false" name="_xlnm._FilterDatabase_1_1_1_1" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
+    <definedName function="false" hidden="false" name="_xlnm._FilterDatabase_1_1_1_1_1" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -1151,21 +1152,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6039215686275"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1764705882353"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5607843137255"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.92549019607843"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2117647058824"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.3607843137255"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.62352941176471"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.0705882352941"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.2470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.6156862745098"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.96862745098039"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2823529411765"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4313725490196"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.66666666666667"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.1137254901961"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.2980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="1" s="2">
@@ -2393,28 +2394,28 @@
   <dimension ref="A1:U262"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M42" activeCellId="0" pane="topLeft" sqref="M42"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7098039215686"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.3098039215686"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1725490196078"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1411764705882"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5843137254902"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.31764705882353"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1764705882353"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.3725490196078"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6274509803922"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2392156862745"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.643137254902"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.34509803921569"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8627450980392"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.443137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -4707,29 +4708,32 @@
       <c r="F57" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G57" s="30" t="n">
-        <v>0.035</v>
+      <c r="G57" s="30" t="inlineStr">
+        <f aca="false">F22</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="H57" s="30" t="inlineStr">
-        <f aca="false">+G57</f>
+        <f aca="false">F9</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="I57" s="30" t="inlineStr">
-        <f aca="false">+H57</f>
+        <f aca="false">F11</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="J57" s="30" t="inlineStr">
-        <f aca="false">+I57</f>
+        <f aca="false">F12</f>
         <is>
           <t/>
         </is>
       </c>
       <c r="K57" s="30" t="inlineStr">
-        <f aca="false">+J57</f>
+        <f aca="false">F21</f>
         <is>
           <t/>
         </is>

</xml_diff>